<commit_message>
complete fastq AMD_ID check & id wrong elements
</commit_message>
<xml_diff>
--- a/Geneious_workflow/01_sample_ID_QC/files/AMD_ID_create_template.xlsx
+++ b/Geneious_workflow/01_sample_ID_QC/files/AMD_ID_create_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eldintalundzic/Desktop/02_Variant Calling TES/Sample ID QC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eldintalundzic/MaRS/Geneious_workflow/01_sample_ID_QC/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC0EB63-EF2B-D44F-99A4-06324D3058DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54ADD91-D500-8345-80CF-E13A0F5DFDA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6080" yWindow="1960" windowWidth="44140" windowHeight="26140" activeTab="2" xr2:uid="{6AAFB199-146B-43F7-A9FF-C3EA2DA729F3}"/>
+    <workbookView xWindow="3200" yWindow="3140" windowWidth="44140" windowHeight="26140" activeTab="2" xr2:uid="{6AAFB199-146B-43F7-A9FF-C3EA2DA729F3}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -2727,7 +2727,7 @@
   <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated to the latest changes
</commit_message>
<xml_diff>
--- a/Geneious_workflow/01_sample_ID_QC/files/AMD_ID_create_template.xlsx
+++ b/Geneious_workflow/01_sample_ID_QC/files/AMD_ID_create_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eldintalundzic/MaRS/Geneious_workflow/01_sample_ID_QC/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marko\Desktop\MaRS\Geneious_workflow\01_sample_ID_QC\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54ADD91-D500-8345-80CF-E13A0F5DFDA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7FE4900-FE0E-490A-88CA-CB9ABC9381A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="3140" windowWidth="44140" windowHeight="26140" activeTab="2" xr2:uid="{6AAFB199-146B-43F7-A9FF-C3EA2DA729F3}"/>
+    <workbookView xWindow="9270" yWindow="3795" windowWidth="33525" windowHeight="15390" xr2:uid="{6AAFB199-146B-43F7-A9FF-C3EA2DA729F3}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="156">
   <si>
     <t>BD19-009</t>
   </si>
@@ -189,9 +189,6 @@
     <t>I</t>
   </si>
   <si>
-    <t>J</t>
-  </si>
-  <si>
     <t>K</t>
   </si>
   <si>
@@ -210,15 +207,9 @@
     <t>N</t>
   </si>
   <si>
-    <t>Quinine + Doxycycline</t>
-  </si>
-  <si>
     <t>O</t>
   </si>
   <si>
-    <t>Atovaquone/Proguanil + Arthemether-Lumafantrine</t>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
@@ -237,9 +228,6 @@
     <t>S</t>
   </si>
   <si>
-    <t>Doxycycline, Malarone, Quinine and Artesunate</t>
-  </si>
-  <si>
     <t>T</t>
   </si>
   <si>
@@ -247,12 +235,6 @@
   </si>
   <si>
     <t>U</t>
-  </si>
-  <si>
-    <t>Atovaquone</t>
-  </si>
-  <si>
-    <t>V</t>
   </si>
   <si>
     <t>W</t>
@@ -356,33 +338,15 @@
     <t>CODE</t>
   </si>
   <si>
-    <t>Drug</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
     <t xml:space="preserve">TREATMENT </t>
   </si>
   <si>
     <t xml:space="preserve">Select marker combo: </t>
   </si>
   <si>
-    <t>k13, crt, mdr1, cytb, dhps, dhfr</t>
-  </si>
-  <si>
     <t xml:space="preserve">dhps, dhfr </t>
   </si>
   <si>
-    <t xml:space="preserve">k13, dhps, dhfr </t>
-  </si>
-  <si>
-    <t xml:space="preserve">k13 </t>
-  </si>
-  <si>
-    <t>k13, crt, mdr1, cytb, dhps, dhfr, pfs47</t>
-  </si>
-  <si>
     <t>pfs47</t>
   </si>
   <si>
@@ -398,24 +362,6 @@
     <t>Marker name loc</t>
   </si>
   <si>
-    <t>k13</t>
-  </si>
-  <si>
-    <t>crt</t>
-  </si>
-  <si>
-    <t>mdr1</t>
-  </si>
-  <si>
-    <t>cytb</t>
-  </si>
-  <si>
-    <t>dhps</t>
-  </si>
-  <si>
-    <t>dhfr</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -446,51 +392,9 @@
     <t>000000100</t>
   </si>
   <si>
-    <t>(AL) Arthemether-Lumafantrine - Coartem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(CQ) Chloroquine </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (CQ+PQ) Chloroquine + Piperaquine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(AL+PQ) Arthemether-Lumafantrine + Piperaquine </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(AL+MQ) Arthemether + Mefloquine(Lariam) </t>
-  </si>
-  <si>
-    <t>(AS+AQ) Artesunate + Amodiaquine </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (AS+SP) Artesunate + Sulphadoxine-Pyrimethamine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (AS+MQ) Artesunate + Mefloquine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (DHA+PQ) Dihydroartemisinin + Piperaquine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (AS+SP+PQ) Artesunate + Sulphadoxine + Pyrimethamine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(AL+MQ+PQ) Arthemether + Mefloquine + Piperaquine </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Malarone) Atovaquone/Proguanil </t>
-  </si>
-  <si>
     <t>Malarone + Doxycycline</t>
   </si>
   <si>
-    <t>Coartem + Artesunate </t>
-  </si>
-  <si>
-    <t>Malarone + Coartem + Artesunate </t>
-  </si>
-  <si>
     <t>AMD_ID</t>
   </si>
   <si>
@@ -576,6 +480,123 @@
   </si>
   <si>
     <t>p</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>Code </t>
+  </si>
+  <si>
+    <t>Arthemether-Lumafantrine (AL)- Coartem</t>
+  </si>
+  <si>
+    <t>Chloroquine (CQ) </t>
+  </si>
+  <si>
+    <t>Chloroquine + Piperaquine (CQ+PQ) </t>
+  </si>
+  <si>
+    <t>Arthemether-Lumafantrine + Piperaquine (AL+PQ)</t>
+  </si>
+  <si>
+    <t>Arthemether + Mefloquine(Lariam) (AL+MQ) </t>
+  </si>
+  <si>
+    <t>Artesunate + Amodiaquine (AS+AQ)</t>
+  </si>
+  <si>
+    <t>Artesunate + Sulfadoxine-Pyrimethamine (AS+SP)</t>
+  </si>
+  <si>
+    <t>Artesunate + Mefloquine (AS+MQ)</t>
+  </si>
+  <si>
+    <t>Dihydroartemisinin + Piperaquine (DHA+PQ)</t>
+  </si>
+  <si>
+    <t>Arthemether + Mefloquine + Piperaquine (AL+MQ+PQ) </t>
+  </si>
+  <si>
+    <t>Atovaquone/Proguanil (Malarone)</t>
+  </si>
+  <si>
+    <t>Doxycycline + Quinine (L + N)</t>
+  </si>
+  <si>
+    <t>Arthemether-Lumafantrine + Atovaquone/Proguanil  (AL + M)</t>
+  </si>
+  <si>
+    <t>Doxycycline + Atovaquone/Proguanil (Malarone) (L + M)</t>
+  </si>
+  <si>
+    <t>Doxycycline, Malarone, Quinine and Artesunate (L + M + N + AS)</t>
+  </si>
+  <si>
+    <t>Coartem + Artesunate + Malarone (AL + AS + M)</t>
+  </si>
+  <si>
+    <t>Arthemether-Lumafantrine (Coartem) + Artesunate (AL + AS) </t>
+  </si>
+  <si>
+    <t>Chloroquine + primaquine (CQ + primaquine)</t>
+  </si>
+  <si>
+    <t>Z </t>
+  </si>
+  <si>
+    <t>Artesunate, Malarone (AS + M)</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Artesunate + Doxycycline (AS +L)</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>Artesunate (AS) only</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Pfk13, Pfcrt, Pfmdr1, Pfcytb, Pfdhps, Pfdhfr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pfk13, Pfdhps, Pfdhfr </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pfdhps, Pfdhfr </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pfk13 </t>
+  </si>
+  <si>
+    <t>Pfk13, Pfcrt, Pfmdr1, Pfcytb, Pfdhps, Pfdhfr, Pfs47</t>
+  </si>
+  <si>
+    <t>Pfs47</t>
+  </si>
+  <si>
+    <t>Pfk13</t>
+  </si>
+  <si>
+    <t>Pfcrt</t>
+  </si>
+  <si>
+    <t>Pfmdr1</t>
+  </si>
+  <si>
+    <t>Pfcytb</t>
+  </si>
+  <si>
+    <t>Pfdhps</t>
+  </si>
+  <si>
+    <t>Pfdhfr</t>
   </si>
 </sst>
 </file>
@@ -931,7 +952,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -1170,6 +1191,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1177,13 +1209,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1192,16 +1224,15 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
@@ -1222,12 +1253,11 @@
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1249,21 +1279,18 @@
     <xf numFmtId="0" fontId="25" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="17" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="4" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1277,7 +1304,6 @@
     <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="29" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1357,6 +1383,12 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1366,6 +1398,124 @@
     <cellStyle name="Normal 2" xfId="3" xr:uid="{636481B1-F3DE-0B41-8396-4FE774CD0495}"/>
   </cellStyles>
   <dxfs count="18">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <name val="Rockwell"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <name val="Rockwell"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <name val="Rockwell"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1492,65 +1642,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color theme="4" tint="0.39997558519241921"/>
@@ -1566,25 +1657,6 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1617,46 +1689,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1765,23 +1797,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{248AFE6F-2966-5B4D-8228-BB95EB12B149}" name="Treatment" displayName="Treatment" ref="A1:B25" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
-  <autoFilter ref="A1:B25" xr:uid="{F2224F94-D8A2-4D12-A1E1-00B3307BEE1A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{248AFE6F-2966-5B4D-8228-BB95EB12B149}" name="Treatment" displayName="Treatment" ref="A1:B27" totalsRowShown="0" headerRowDxfId="17" dataDxfId="0" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+  <autoFilter ref="A1:B27" xr:uid="{F2224F94-D8A2-4D12-A1E1-00B3307BEE1A}"/>
   <tableColumns count="2">
-    <tableColumn id="2" xr3:uid="{B5FBA0FD-639D-5540-ACE3-297BFA879D77}" name="Drug" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{89EE1570-2AD1-3644-AC7E-E360E2494C94}" name="Code" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{B5FBA0FD-639D-5540-ACE3-297BFA879D77}" name="Treatment" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{89EE1570-2AD1-3644-AC7E-E360E2494C94}" name="Code " dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{70AAFBD9-5D6A-6448-8E96-A7341A8797AD}" name="Markers" displayName="Markers" ref="A1:C25" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5" tableBorderDxfId="3" totalsRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{70AAFBD9-5D6A-6448-8E96-A7341A8797AD}" name="Markers" displayName="Markers" ref="A1:C25" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="A1:C25" xr:uid="{F2224F94-D8A2-4D12-A1E1-00B3307BEE1A}"/>
   <tableColumns count="3">
-    <tableColumn id="2" xr3:uid="{3D8943B6-3C35-8D4E-B7EA-19AB9FEFAF2E}" name="molecular markers" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{3D8943B6-3C35-8D4E-B7EA-19AB9FEFAF2E}" name="molecular markers" dataDxfId="8"/>
     <tableColumn id="1" xr3:uid="{9DD6753C-E602-4D40-8CFC-9A2262EA4965}" name="bit code"/>
-    <tableColumn id="3" xr3:uid="{40AF72EE-A935-774C-882A-4B6CDF404A1A}" name="code" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{40AF72EE-A935-774C-882A-4B6CDF404A1A}" name="code" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2086,51 +2118,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD02E6BE-1C57-DC4B-8719-C115FD8E1D00}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.6640625" customWidth="1"/>
+    <col min="1" max="1" width="52.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="92" customHeight="1" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="92.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="177" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" ht="177" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="53" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="53.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>26</v>
       </c>
@@ -2147,145 +2179,142 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52AD23B7-C55B-5C4F-BCF0-4AC731D06C05}">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView zoomScale="144" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="44"/>
-    <col min="4" max="4" width="10.83203125" style="44" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" style="44" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" style="44" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5" style="44" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" style="44" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5" style="44" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" style="44" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" style="44" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" style="44" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.625" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="41"/>
+    <col min="4" max="4" width="10.875" style="41" customWidth="1"/>
+    <col min="5" max="5" width="16.875" style="41" customWidth="1"/>
+    <col min="6" max="6" width="15.125" style="41" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" style="41" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.625" style="41" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" style="41" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.375" style="41" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.625" style="41" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.375" style="41" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.375" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="45.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="45.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B1" s="5"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-    </row>
-    <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+    </row>
+    <row r="2" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="74" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="75"/>
+      <c r="E2" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" s="78" t="s">
-        <v>78</v>
-      </c>
-      <c r="D2" s="79"/>
-      <c r="E2" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="F2" s="48"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49" t="s">
-        <v>123</v>
-      </c>
-      <c r="E3" s="49" t="s">
-        <v>124</v>
-      </c>
-      <c r="F3" s="50" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="str" cm="1">
-        <f t="array" ref="A4:B4">_xlfn._xlws.FILTER(Treatment[],Treatment[Drug]=B2,"Nothing found")</f>
-        <v>Malarone + Doxycycline</v>
-      </c>
-      <c r="B4" s="43" t="str">
-        <v>S</v>
-      </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51" t="str" cm="1">
+      <c r="F2" s="45"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="39" t="str" cm="1">
+        <f t="array" ref="A4">_xlfn._xlws.FILTER(Treatment[],Treatment[Treatment]=B2,"Nothing found")</f>
+        <v>Nothing found</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47" t="str" cm="1">
         <f t="array" ref="D4:F4">_xlfn._xlws.FILTER(Markers[],Markers[molecular markers]=E2,"nothing found")</f>
-        <v>pfs47</v>
-      </c>
-      <c r="E4" s="51" t="str">
+        <v>Pfs47</v>
+      </c>
+      <c r="E4" s="47" t="str">
         <v>000000100</v>
       </c>
-      <c r="F4" s="52">
+      <c r="F4" s="48">
         <v>4</v>
       </c>
-      <c r="G4" s="44" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="56" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" s="57" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="58" t="s">
+      <c r="G4" s="41" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="J6" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="58" t="s">
+      <c r="K6" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="58" t="s">
+      <c r="L6" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="58" t="s">
-        <v>62</v>
-      </c>
-      <c r="G6" s="58" t="s">
-        <v>63</v>
-      </c>
-      <c r="H6" s="58" t="s">
-        <v>71</v>
-      </c>
-      <c r="I6" s="58" t="s">
-        <v>64</v>
-      </c>
-      <c r="J6" s="58" t="s">
-        <v>65</v>
-      </c>
-      <c r="K6" s="58" t="s">
-        <v>66</v>
-      </c>
-      <c r="L6" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="M6" s="64" t="s">
-        <v>120</v>
-      </c>
-      <c r="N6" s="63" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="M6" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="N6" s="59" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>0</v>
       </c>
@@ -2315,7 +2344,7 @@
         <v>6</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="L7" s="9">
         <v>1</v>
@@ -2329,7 +2358,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>7</v>
       </c>
@@ -2359,7 +2388,7 @@
         <v>6</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="L8" s="9">
         <v>1</v>
@@ -2373,7 +2402,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
@@ -2403,7 +2432,7 @@
         <v>6</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="L9" s="9">
         <v>1</v>
@@ -2417,7 +2446,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
@@ -2447,7 +2476,7 @@
         <v>6</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="L10" s="9">
         <v>1</v>
@@ -2460,11 +2489,8 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
@@ -2494,7 +2520,7 @@
         <v>6</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="L11" s="9">
         <v>1</v>
@@ -2508,7 +2534,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>15</v>
       </c>
@@ -2538,7 +2564,7 @@
         <v>6</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="L12" s="9">
         <v>1</v>
@@ -2552,7 +2578,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>17</v>
       </c>
@@ -2582,7 +2608,7 @@
         <v>6</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="L13" s="9">
         <v>1</v>
@@ -2596,7 +2622,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>19</v>
       </c>
@@ -2626,7 +2652,7 @@
         <v>6</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="L14" s="9">
         <v>1</v>
@@ -2637,7 +2663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>21</v>
       </c>
@@ -2667,22 +2693,22 @@
         <v>6</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="L15" s="9">
         <v>1</v>
       </c>
-      <c r="M15" s="53" t="s">
-        <v>122</v>
+      <c r="M15" s="49" t="s">
+        <v>90</v>
       </c>
       <c r="N15" s="10">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="N16" s="53" t="s">
-        <v>122</v>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N16" s="49" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2690,10 +2716,10 @@
     <mergeCell ref="C2:D2"/>
   </mergeCells>
   <conditionalFormatting sqref="N7:N15">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
       <formula>20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThan">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2724,149 +2750,142 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF8F6B5C-1385-7E49-8493-A903617FF235}">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScale="144" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="44"/>
-    <col min="4" max="4" width="10.83203125" style="44" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" style="44" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" style="44" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5" style="44" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" style="44" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" style="44" customWidth="1"/>
-    <col min="10" max="10" width="12.5" style="44" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" style="44" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" style="44" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" style="44" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.33203125" style="44" customWidth="1"/>
+    <col min="2" max="2" width="24.625" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="41"/>
+    <col min="4" max="4" width="10.875" style="41" customWidth="1"/>
+    <col min="5" max="5" width="16.875" style="41" customWidth="1"/>
+    <col min="6" max="6" width="15.125" style="41" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" style="41" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.625" style="41" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.625" style="41" customWidth="1"/>
+    <col min="10" max="10" width="12.5" style="41" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.375" style="41" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.625" style="41" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.375" style="41" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.375" style="41" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="45.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="45.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B1" s="5"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-    </row>
-    <row r="2" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" s="78" t="s">
-        <v>78</v>
-      </c>
-      <c r="D2" s="79"/>
-      <c r="E2" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" s="48"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49" t="s">
-        <v>123</v>
-      </c>
-      <c r="E3" s="49" t="s">
-        <v>124</v>
-      </c>
-      <c r="F3" s="50" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="str" cm="1">
-        <f t="array" ref="A4:B4">_xlfn._xlws.FILTER(Treatment[],Treatment[Drug]=B2,"Nothing found")</f>
-        <v>Malarone + Doxycycline</v>
-      </c>
-      <c r="B4" s="43" t="str">
-        <v>S</v>
-      </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51" t="str" cm="1">
-        <f t="array" ref="D4:F4">_xlfn._xlws.FILTER(Markers[],Markers[molecular markers]=E2,"nothing found")</f>
-        <v xml:space="preserve">dhps, dhfr </v>
-      </c>
-      <c r="E4" s="51" t="str">
-        <v>000011000</v>
-      </c>
-      <c r="F4" s="55">
-        <v>24</v>
-      </c>
-      <c r="G4" s="44" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="56" t="s">
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+    </row>
+    <row r="2" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="74" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="D2" s="75"/>
+      <c r="E2" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="45"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="B3" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="39" t="str" cm="1">
+        <f t="array" ref="A4">_xlfn._xlws.FILTER(Treatment[],Treatment[Treatment]=B2,"Nothing found")</f>
+        <v>Nothing found</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47" t="str" cm="1">
+        <f t="array" ref="D4">_xlfn._xlws.FILTER(Markers[],Markers[molecular markers]=E2,"nothing found")</f>
+        <v>nothing found</v>
+      </c>
+      <c r="E4" s="47"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="41" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" s="56" t="s">
+        <v>102</v>
+      </c>
+      <c r="J6" s="57" t="s">
+        <v>95</v>
+      </c>
+      <c r="K6" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="58" t="s">
+      <c r="L6" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="58" t="s">
+      <c r="M6" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="58" t="s">
-        <v>62</v>
-      </c>
-      <c r="G6" s="58" t="s">
-        <v>63</v>
-      </c>
-      <c r="H6" s="59" t="s">
-        <v>71</v>
-      </c>
-      <c r="I6" s="60" t="s">
-        <v>134</v>
-      </c>
-      <c r="J6" s="61" t="s">
-        <v>127</v>
-      </c>
-      <c r="K6" s="58" t="s">
-        <v>65</v>
-      </c>
-      <c r="L6" s="58" t="s">
-        <v>66</v>
-      </c>
-      <c r="M6" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="N6" s="62" t="s">
-        <v>120</v>
-      </c>
-      <c r="O6" s="63" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="N6" s="58" t="s">
+        <v>88</v>
+      </c>
+      <c r="O6" s="59" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>0</v>
       </c>
@@ -2881,25 +2900,25 @@
         <v>2</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>3</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>135</v>
+        <v>103</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="K7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
       <c r="M7" s="9">
         <v>1</v>
@@ -2913,7 +2932,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>7</v>
       </c>
@@ -2928,25 +2947,25 @@
         <v>2</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>3</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>136</v>
+        <v>104</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="K8" s="9" t="s">
         <v>6</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
       <c r="M8" s="9">
         <v>1</v>
@@ -2960,7 +2979,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
@@ -2975,25 +2994,25 @@
         <v>2</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>3</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
       <c r="K9" s="9" t="s">
         <v>6</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
       <c r="M9" s="9">
         <v>1</v>
@@ -3007,7 +3026,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
@@ -3022,25 +3041,25 @@
         <v>2</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>3</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="K10" s="9" t="s">
         <v>6</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
       <c r="M10" s="9">
         <v>1</v>
@@ -3053,11 +3072,8 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
@@ -3072,25 +3088,25 @@
         <v>2</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>3</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="K11" s="9" t="s">
         <v>6</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
       <c r="M11" s="9">
         <v>1</v>
@@ -3104,7 +3120,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>15</v>
       </c>
@@ -3119,25 +3135,25 @@
         <v>2</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>3</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="K12" s="9" t="s">
         <v>6</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
       <c r="M12" s="9">
         <v>1</v>
@@ -3151,7 +3167,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>17</v>
       </c>
@@ -3166,25 +3182,25 @@
         <v>2</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>3</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
       <c r="K13" s="9" t="s">
         <v>6</v>
       </c>
       <c r="L13" s="9" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
       <c r="M13" s="9">
         <v>1</v>
@@ -3198,7 +3214,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>19</v>
       </c>
@@ -3213,25 +3229,25 @@
         <v>2</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>3</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>142</v>
+        <v>110</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="K14" s="9" t="s">
         <v>6</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
       <c r="M14" s="9">
         <v>1</v>
@@ -3242,7 +3258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>21</v>
       </c>
@@ -3257,40 +3273,40 @@
         <v>2</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="G15" s="9" t="s">
         <v>3</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="K15" s="9" t="s">
         <v>6</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
       <c r="M15" s="9">
         <v>1</v>
       </c>
-      <c r="N15" s="54" t="s">
-        <v>122</v>
+      <c r="N15" s="50" t="s">
+        <v>90</v>
       </c>
       <c r="O15" s="10">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="O16" s="53" t="s">
-        <v>122</v>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O16" s="49" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -3298,10 +3314,10 @@
     <mergeCell ref="C2:D2"/>
   </mergeCells>
   <conditionalFormatting sqref="O7:O15">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
       <formula>20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3332,260 +3348,275 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C37955B0-227B-104F-9235-33E61CAD4B32}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView zoomScale="165" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.1640625" style="70" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" style="70" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" style="12" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" style="20" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.1640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.6640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" style="20"/>
-    <col min="11" max="16384" width="8.83203125" style="12"/>
+    <col min="1" max="1" width="47.25" style="66" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.625" style="66" customWidth="1"/>
+    <col min="3" max="3" width="14.875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="10.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="11.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.375" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="71" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" s="71" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="65" t="s">
-        <v>105</v>
-      </c>
-      <c r="B2" s="66" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="67" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="67" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="61" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="67" t="s">
-        <v>106</v>
-      </c>
-      <c r="B3" s="68" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="20"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="63" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="64" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="65" t="s">
-        <v>107</v>
-      </c>
-      <c r="B4" s="66" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="61" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-    </row>
-    <row r="5" spans="1:9" ht="26" x14ac:dyDescent="0.2">
-      <c r="A5" s="67" t="s">
-        <v>108</v>
-      </c>
-      <c r="B5" s="68" t="s">
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="63" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="24"/>
-      <c r="I5" s="25"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="65" t="s">
-        <v>109</v>
-      </c>
-      <c r="B6" s="66" t="s">
+      <c r="D5" s="22"/>
+      <c r="I5" s="23"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="61" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="I6" s="25"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="67" t="s">
-        <v>110</v>
-      </c>
-      <c r="B7" s="68" t="s">
+      <c r="D6" s="22"/>
+      <c r="I6" s="23"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="63" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="I7" s="25"/>
-    </row>
-    <row r="8" spans="1:9" ht="26" x14ac:dyDescent="0.2">
-      <c r="A8" s="65" t="s">
-        <v>111</v>
-      </c>
-      <c r="B8" s="66" t="s">
+      <c r="D7" s="22"/>
+      <c r="I7" s="23"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="61" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="I8" s="25"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="67" t="s">
-        <v>112</v>
-      </c>
-      <c r="B9" s="68" t="s">
+      <c r="D8" s="22"/>
+      <c r="I8" s="23"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="63" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="I9" s="25"/>
-    </row>
-    <row r="10" spans="1:9" ht="26" x14ac:dyDescent="0.2">
-      <c r="A10" s="65" t="s">
-        <v>113</v>
-      </c>
-      <c r="B10" s="66" t="s">
+      <c r="D9" s="22"/>
+      <c r="I9" s="23"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="61" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="24"/>
-    </row>
-    <row r="11" spans="1:9" ht="26" x14ac:dyDescent="0.2">
-      <c r="A11" s="67" t="s">
-        <v>114</v>
-      </c>
-      <c r="B11" s="68" t="s">
+      <c r="D10" s="22"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="63" t="s">
+        <v>128</v>
+      </c>
+      <c r="B11" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="24"/>
-    </row>
-    <row r="12" spans="1:9" ht="26" x14ac:dyDescent="0.2">
-      <c r="A12" s="65" t="s">
-        <v>115</v>
-      </c>
-      <c r="B12" s="66" t="s">
+      <c r="D11" s="22"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="24"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="67" t="s">
+      <c r="B12" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="68" t="s">
+      <c r="D12" s="22"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="63" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="24"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="65" t="s">
-        <v>116</v>
-      </c>
-      <c r="B14" s="66" t="s">
+      <c r="D13" s="22"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="24"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="67" t="s">
+      <c r="B14" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="68" t="s">
+      <c r="D14" s="22"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="63" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="24"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="65" t="s">
+      <c r="D15" s="22"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="61" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="66" t="s">
+      <c r="D16" s="22"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="24"/>
-    </row>
-    <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A17" s="67" t="s">
+      <c r="B17" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="68" t="s">
+      <c r="D17" s="22"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="24"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="65" t="s">
+      <c r="B18" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="66" t="s">
+      <c r="D18" s="22"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="63" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="24"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="67" t="s">
+      <c r="D19" s="22"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="61" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="68" t="s">
+      <c r="D20" s="22"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="24"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="65" t="s">
-        <v>117</v>
-      </c>
-      <c r="B20" s="66" t="s">
+      <c r="B21" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="24"/>
-    </row>
-    <row r="21" spans="1:4" ht="27" x14ac:dyDescent="0.2">
-      <c r="A21" s="69" t="s">
+      <c r="D21" s="22"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="61" t="s">
+        <v>134</v>
+      </c>
+      <c r="B22" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="68" t="s">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="63" t="s">
+        <v>135</v>
+      </c>
+      <c r="B23" s="64" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="24"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="65" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="66" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="67" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="68" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="65" t="s">
-        <v>119</v>
-      </c>
-      <c r="B24" s="66" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="67" t="s">
-        <v>118</v>
-      </c>
-      <c r="B25" s="68" t="s">
-        <v>57</v>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="76" t="s">
+        <v>136</v>
+      </c>
+      <c r="B24" s="77" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="63" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" s="64" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="76" t="s">
+        <v>140</v>
+      </c>
+      <c r="B26" s="77" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="63" t="s">
+        <v>142</v>
+      </c>
+      <c r="B27" s="64" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -3606,136 +3637,144 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F67332F-5BB4-1F48-9C47-C26803FFCC92}">
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.83203125" style="12"/>
+    <col min="1" max="16384" width="8.875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="str" cm="1">
-        <f t="array" ref="A1:A24">_xlfn.UNIQUE(Treatment[Drug])</f>
-        <v>(AL) Arthemether-Lumafantrine - Coartem</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="str">
-        <v xml:space="preserve">(CQ) Chloroquine </v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="str">
-        <v xml:space="preserve"> (CQ+PQ) Chloroquine + Piperaquine</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="str">
-        <v xml:space="preserve">(AL+PQ) Arthemether-Lumafantrine + Piperaquine </v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="str">
-        <v xml:space="preserve">(AL+MQ) Arthemether + Mefloquine(Lariam) </v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="str">
-        <v>(AS+AQ) Artesunate + Amodiaquine </v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="str">
-        <v xml:space="preserve"> (AS+SP) Artesunate + Sulphadoxine-Pyrimethamine</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="str">
-        <v xml:space="preserve"> (AS+MQ) Artesunate + Mefloquine</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="str">
-        <v xml:space="preserve"> (DHA+PQ) Dihydroartemisinin + Piperaquine</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="str">
-        <v xml:space="preserve"> (AS+SP+PQ) Artesunate + Sulphadoxine + Pyrimethamine</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="str">
-        <v xml:space="preserve">(AL+MQ+PQ) Arthemether + Mefloquine + Piperaquine </v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="str">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="str" cm="1">
+        <f t="array" ref="A1:A26">_xlfn.UNIQUE(Treatment[Treatment])</f>
+        <v>Arthemether-Lumafantrine (AL)- Coartem</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="str">
+        <v>Chloroquine (CQ) </v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="str">
+        <v>Chloroquine + Piperaquine (CQ+PQ) </v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="str">
+        <v>Arthemether-Lumafantrine + Piperaquine (AL+PQ)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="str">
+        <v>Arthemether + Mefloquine(Lariam) (AL+MQ) </v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="str">
+        <v>Artesunate + Amodiaquine (AS+AQ)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="str">
+        <v>Artesunate + Sulfadoxine-Pyrimethamine (AS+SP)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="str">
+        <v>Artesunate + Mefloquine (AS+MQ)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="str">
+        <v>Dihydroartemisinin + Piperaquine (DHA+PQ)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="str">
+        <v>Arthemether + Mefloquine + Piperaquine (AL+MQ+PQ) </v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="str">
         <v>Doxycycline</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="str">
-        <v xml:space="preserve">(Malarone) Atovaquone/Proguanil </v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="str">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="str">
+        <v>Atovaquone/Proguanil (Malarone)</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="str">
         <v>Quinine</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="str">
-        <v>Quinine + Doxycycline</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="str">
-        <v>Atovaquone/Proguanil + Arthemether-Lumafantrine</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="str">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="str">
+        <v>Doxycycline + Quinine (L + N)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="str">
+        <v>Arthemether-Lumafantrine + Atovaquone/Proguanil  (AL + M)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="str">
         <v>Mefloquine</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="str">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="str">
         <v>Vanomycin and Rocephin</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="str">
-        <v>Malarone + Doxycycline</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="str">
-        <v>Doxycycline, Malarone, Quinine and Artesunate</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="12" t="str">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="str">
+        <v>Doxycycline + Atovaquone/Proguanil (Malarone) (L + M)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="str">
+        <v>Doxycycline, Malarone, Quinine and Artesunate (L + M + N + AS)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="str">
         <v>Hydroxychloroquine</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="str">
-        <v>Atovaquone</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="12" t="str">
-        <v>Malarone + Coartem + Artesunate </v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="12" t="str">
-        <v>Coartem + Artesunate </v>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="str">
+        <v>Coartem + Artesunate + Malarone (AL + AS + M)</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="str">
+        <v>Arthemether-Lumafantrine (Coartem) + Artesunate (AL + AS) </v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="str">
+        <v>Chloroquine + primaquine (CQ + primaquine)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="str">
+        <v>Artesunate, Malarone (AS + M)</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="str">
+        <v>Artesunate + Doxycycline (AS +L)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="str">
+        <v>Artesunate (AS) only</v>
       </c>
     </row>
   </sheetData>
@@ -3748,300 +3787,299 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" style="19" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" style="20" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="10" style="20" customWidth="1"/>
-    <col min="10" max="14" width="10" style="12" customWidth="1"/>
-    <col min="15" max="16384" width="8.83203125" style="12"/>
+    <col min="1" max="1" width="37.75" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.375" style="18" customWidth="1"/>
+    <col min="3" max="3" width="23.375" style="18" customWidth="1"/>
+    <col min="4" max="4" width="17.125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="11.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="14" width="10" style="11" customWidth="1"/>
+    <col min="15" max="16384" width="8.875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="72" t="s">
-        <v>85</v>
-      </c>
-      <c r="C1" s="72" t="s">
-        <v>86</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="F1" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G1" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="J1" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="K1" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="L1" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="M1" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="N1" s="29" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="26" t="s">
+    <row r="1" spans="1:14" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="68" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="68" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="68" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="M1" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="74">
+      <c r="N1" s="27" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="17.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="70">
         <v>111111000</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="13">
         <f>BIN2DEC(Markers[[#This Row],[bit code]])</f>
         <v>504</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="F2" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="G2" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="H2" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="I2" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="J2" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="K2" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="L2" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="M2" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="N2" s="31" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="76" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" s="37">
+      <c r="D2" s="20"/>
+      <c r="E2" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="M2" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="N2" s="29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="72" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="34">
         <f>BIN2DEC(Markers[[#This Row],[bit code]])</f>
         <v>280</v>
       </c>
-      <c r="E3" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="F3" s="33">
+      <c r="E3" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" s="30">
         <v>0</v>
       </c>
-      <c r="G3" s="33">
+      <c r="G3" s="30">
         <v>0</v>
       </c>
-      <c r="H3" s="33">
+      <c r="H3" s="30">
         <v>0</v>
       </c>
-      <c r="I3" s="33">
+      <c r="I3" s="30">
         <v>0</v>
       </c>
-      <c r="J3" s="33">
+      <c r="J3" s="30">
         <v>0</v>
       </c>
-      <c r="K3" s="33">
+      <c r="K3" s="30">
         <v>0</v>
       </c>
-      <c r="L3" s="33">
+      <c r="L3" s="30">
         <v>1</v>
       </c>
-      <c r="M3" s="33">
+      <c r="M3" s="30">
         <v>0</v>
       </c>
-      <c r="N3" s="33">
+      <c r="N3" s="30">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="77" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="13">
         <f>BIN2DEC(Markers[[#This Row],[bit code]])</f>
         <v>24</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="F4" s="36" t="str">
+      <c r="D4" s="21"/>
+      <c r="E4" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="33" t="str">
         <f>_xlfn.CONCAT(F3:N3)</f>
         <v>000000100</v>
       </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="76" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="37">
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" s="72" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="34">
         <f>BIN2DEC(Markers[[#This Row],[bit code]])</f>
         <v>256</v>
       </c>
-      <c r="H5" s="25"/>
-    </row>
-    <row r="6" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="B6" s="73" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" s="14">
+      <c r="H5" s="23"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="69" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="13">
         <f>BIN2DEC(Markers[[#This Row],[bit code]])</f>
         <v>508</v>
       </c>
-      <c r="E6" s="35"/>
-      <c r="H6" s="25"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7" s="75" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7" s="37">
+      <c r="E6" s="32"/>
+      <c r="H6" s="23"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" s="71" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="34">
         <f>BIN2DEC(Markers[[#This Row],[bit code]])</f>
         <v>4</v>
       </c>
-      <c r="H7" s="25"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="17"/>
-      <c r="H8" s="25"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="H9" s="25"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="17"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="17"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="16"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="17"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="16"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="17"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="17"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="17"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="16"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="17"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="16"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="17"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
+      <c r="H7" s="23"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="16"/>
+      <c r="H8" s="23"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="H9" s="23"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="16"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="16"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="16"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="15"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="16"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="16"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="16"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="15"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="16"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="15"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="16"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4075,45 +4113,45 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" style="12" customWidth="1"/>
-    <col min="2" max="16384" width="8.83203125" style="12"/>
+    <col min="1" max="1" width="31.625" style="11" customWidth="1"/>
+    <col min="2" max="16384" width="8.875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="str" cm="1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="str" cm="1">
         <f t="array" ref="A1:A7">_xlfn.UNIQUE(Markers[molecular markers])</f>
-        <v>k13, crt, mdr1, cytb, dhps, dhfr</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="str">
-        <v xml:space="preserve">k13, dhps, dhfr </v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="str">
-        <v xml:space="preserve">dhps, dhfr </v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="str">
-        <v xml:space="preserve">k13 </v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="str">
-        <v>k13, crt, mdr1, cytb, dhps, dhfr, pfs47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="str">
-        <v>pfs47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="12">
+        <v>Pfk13, Pfcrt, Pfmdr1, Pfcytb, Pfdhps, Pfdhfr</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="str">
+        <v xml:space="preserve">Pfk13, Pfdhps, Pfdhfr </v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="str">
+        <v xml:space="preserve">Pfdhps, Pfdhfr </v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="str">
+        <v xml:space="preserve">Pfk13 </v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="str">
+        <v>Pfk13, Pfcrt, Pfmdr1, Pfcytb, Pfdhps, Pfdhfr, Pfs47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="str">
+        <v>Pfs47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
         <v>0</v>
       </c>
     </row>

</xml_diff>